<commit_message>
Modified Figure3C and Tobacco Figure.
</commit_message>
<xml_diff>
--- a/Tobacco_Data/Dat/Exp1.xlsx
+++ b/Tobacco_Data/Dat/Exp1.xlsx
@@ -14253,8 +14253,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001DC0865C238FB942843D9D158E0C200F" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f4736a172056a9a0292bfc298dbe24f9">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b99972df-dc4a-4b19-b0f2-4adcf421e618" xmlns:ns3="973adfc0-f7c5-479e-a81b-ae331b538917" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a89f3ae39b45fe2b033d473a748749ac" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001DC0865C238FB942843D9D158E0C200F" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c018369d16a63c6a7fad3928115aed9">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b99972df-dc4a-4b19-b0f2-4adcf421e618" xmlns:ns3="973adfc0-f7c5-479e-a81b-ae331b538917" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="443c1f5022f689a902b3653a38b2c685" ns2:_="" ns3:_="">
     <xsd:import namespace="b99972df-dc4a-4b19-b0f2-4adcf421e618"/>
     <xsd:import namespace="973adfc0-f7c5-479e-a81b-ae331b538917"/>
     <xsd:element name="properties">
@@ -14276,6 +14276,10 @@
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns2:Search" minOccurs="0"/>
+                <xsd:element ref="ns2:Preview" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -14352,6 +14356,16 @@
         <xsd:restriction base="dms:Lookup"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="Preview" ma:index="22" nillable="true" ma:displayName="Preview" ma:format="Thumbnail" ma:internalName="Preview">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="25" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="973adfc0-f7c5-479e-a81b-ae331b538917" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -14366,6 +14380,32 @@
           </xsd:extension>
         </xsd:complexContent>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="23" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="24" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -14476,10 +14516,27 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Search xmlns="b99972df-dc4a-4b19-b0f2-4adcf421e618" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b99972df-dc4a-4b19-b0f2-4adcf421e618">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="973adfc0-f7c5-479e-a81b-ae331b538917" xsi:nil="true"/>
+    <Preview xmlns="b99972df-dc4a-4b19-b0f2-4adcf421e618" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{832A7076-6356-4389-90B1-2C99084BCDD3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DD38513-6394-4793-BDD5-C2C9A5CCD1D1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF99AAC8-627A-4336-ADBE-5C644E1C6869}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03866050-992A-4585-AC27-C9D86FDBA3CB}"/>
 </file>
</xml_diff>